<commit_message>
lots of glms and spatial correlograms
</commit_message>
<xml_diff>
--- a/GLM/glm summary 9-3-2014.xlsx
+++ b/GLM/glm summary 9-3-2014.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="133">
   <si>
     <t>Estimate</t>
   </si>
@@ -527,6 +527,21 @@
   <si>
     <t>Nagelkerke adjusted</t>
   </si>
+  <si>
+    <t>Fppres</t>
+  </si>
+  <si>
+    <t>cond + longitude + secchi + totalP</t>
+  </si>
+  <si>
+    <t>cond + longitude + secchi + totalP + lakes_1km + pH + latitude + dist_occupied + lakes_10km + waterfowl + boatlaunch + size</t>
+  </si>
+  <si>
+    <t>FP presence/absence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STILL NEED TO ADD FP PRESENCE </t>
+  </si>
 </sst>
 </file>
 
@@ -536,7 +551,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -701,6 +716,14 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1082,7 +1105,7 @@
     <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1131,6 +1154,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1176,7 +1204,37 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1508,7 +1566,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1928,15 +1986,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L67"/>
+  <dimension ref="A1:P88"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J75" sqref="J75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="5" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="10" customWidth="1"/>
     <col min="9" max="9" width="4.28515625" customWidth="1"/>
@@ -3449,128 +3507,707 @@
         <v>0.18390799999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A57" s="9" t="s">
+    <row r="56" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G57" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H57" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J57" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K57" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L57" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" s="33">
+        <v>-3.646201</v>
+      </c>
+      <c r="C58" s="33">
+        <v>1.318605</v>
+      </c>
+      <c r="D58" s="33">
+        <v>1.327288</v>
+      </c>
+      <c r="E58" s="33">
+        <v>2.7469999999999999</v>
+      </c>
+      <c r="F58" s="33">
+        <v>6.0099999999999997E-3</v>
+      </c>
+      <c r="G58" s="2">
+        <v>-6.2476381999999999</v>
+      </c>
+      <c r="H58" s="2">
+        <v>-1.0447637999999999</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K58" s="2">
+        <v>1</v>
+      </c>
+      <c r="L58" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="33">
+        <v>3.5329160000000002</v>
+      </c>
+      <c r="C59" s="33">
+        <v>1.2057100000000001</v>
+      </c>
+      <c r="D59" s="33">
+        <v>1.213508</v>
+      </c>
+      <c r="E59" s="33">
+        <v>2.911</v>
+      </c>
+      <c r="F59" s="33">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="G59" s="2">
+        <v>1.1544836999999999</v>
+      </c>
+      <c r="H59" s="2">
+        <v>5.9113480000000003</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K59" s="2">
+        <v>1</v>
+      </c>
+      <c r="L59" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" s="33">
+        <v>0.54410599999999998</v>
+      </c>
+      <c r="C60" s="33">
+        <v>0.80477100000000001</v>
+      </c>
+      <c r="D60" s="33">
+        <v>0.80750100000000002</v>
+      </c>
+      <c r="E60" s="33">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="F60" s="33">
+        <v>0.50043000000000004</v>
+      </c>
+      <c r="G60" s="2">
+        <v>-0.42544359999999998</v>
+      </c>
+      <c r="H60" s="2">
+        <v>2.7754997000000001</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K60" s="2">
+        <v>1</v>
+      </c>
+      <c r="L60" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" s="33">
+        <v>-2.7370329999999998</v>
+      </c>
+      <c r="C61" s="33">
+        <v>1.2762169999999999</v>
+      </c>
+      <c r="D61" s="33">
+        <v>1.2853889999999999</v>
+      </c>
+      <c r="E61" s="33">
+        <v>2.129</v>
+      </c>
+      <c r="F61" s="33">
+        <v>3.3230000000000003E-2</v>
+      </c>
+      <c r="G61" s="2">
+        <v>-5.2563493000000001</v>
+      </c>
+      <c r="H61" s="2">
+        <v>-0.21771599999999999</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K61" s="2">
+        <v>0.46</v>
+      </c>
+      <c r="L61" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B62" s="33">
+        <v>4.739579</v>
+      </c>
+      <c r="C62" s="33">
+        <v>1.5687409999999999</v>
+      </c>
+      <c r="D62" s="33">
+        <v>1.5799730000000001</v>
+      </c>
+      <c r="E62" s="33">
+        <v>3</v>
+      </c>
+      <c r="F62" s="33">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="G62" s="2">
+        <v>1.6428894999999999</v>
+      </c>
+      <c r="H62" s="2">
+        <v>7.8362691</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K62" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="L62" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63" s="33">
+        <v>-0.33143099999999998</v>
+      </c>
+      <c r="C63" s="33">
+        <v>0.63272399999999995</v>
+      </c>
+      <c r="D63" s="33">
+        <v>0.63486900000000002</v>
+      </c>
+      <c r="E63" s="33">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="F63" s="33">
+        <v>0.60163999999999995</v>
+      </c>
+      <c r="G63" s="2">
+        <v>-2.4361264999999999</v>
+      </c>
+      <c r="H63" s="2">
+        <v>0.49967289999999998</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K63" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="L63" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" s="33">
+        <v>0.40556999999999999</v>
+      </c>
+      <c r="C64" s="33">
+        <v>1.015307</v>
+      </c>
+      <c r="D64" s="33">
+        <v>1.018883</v>
+      </c>
+      <c r="E64" s="33">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="F64" s="33">
+        <v>0.69059000000000004</v>
+      </c>
+      <c r="G64" s="2">
+        <v>-1.1825922</v>
+      </c>
+      <c r="H64" s="2">
+        <v>4.5699639999999997</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K64" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="L64" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" s="33">
+        <v>-0.24573200000000001</v>
+      </c>
+      <c r="C65" s="33">
+        <v>0.60241800000000001</v>
+      </c>
+      <c r="D65" s="33">
+        <v>0.60433599999999998</v>
+      </c>
+      <c r="E65" s="33">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="F65" s="33">
+        <v>0.68428999999999995</v>
+      </c>
+      <c r="G65" s="2">
+        <v>-2.6903693</v>
+      </c>
+      <c r="H65" s="2">
+        <v>0.65005389999999996</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K65" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="L65" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B66" s="33">
+        <v>0.18145800000000001</v>
+      </c>
+      <c r="C66" s="33">
+        <v>0.57772000000000001</v>
+      </c>
+      <c r="D66" s="33">
+        <v>0.57954799999999995</v>
+      </c>
+      <c r="E66" s="33">
+        <v>0.313</v>
+      </c>
+      <c r="F66" s="33">
+        <v>0.75419999999999998</v>
+      </c>
+      <c r="G66" s="2">
+        <v>-0.80408670000000004</v>
+      </c>
+      <c r="H66" s="2">
+        <v>3.1359618999999999</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K66" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="L66" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B67" s="33">
+        <v>0.18346299999999999</v>
+      </c>
+      <c r="C67" s="33">
+        <v>0.59925499999999998</v>
+      </c>
+      <c r="D67" s="33">
+        <v>0.601329</v>
+      </c>
+      <c r="E67" s="33">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="F67" s="33">
+        <v>0.76029000000000002</v>
+      </c>
+      <c r="G67" s="2">
+        <v>-0.92119720000000005</v>
+      </c>
+      <c r="H67" s="2">
+        <v>3.2819623999999998</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K67" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="L67" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" s="33">
+        <v>0.11201999999999999</v>
+      </c>
+      <c r="C68" s="33">
+        <v>0.44223200000000001</v>
+      </c>
+      <c r="D68" s="33">
+        <v>0.443913</v>
+      </c>
+      <c r="E68" s="33">
+        <v>0.252</v>
+      </c>
+      <c r="F68" s="33">
+        <v>0.80076999999999998</v>
+      </c>
+      <c r="G68" s="2">
+        <v>-0.90429159999999997</v>
+      </c>
+      <c r="H68" s="2">
+        <v>2.7630219999999999</v>
+      </c>
+      <c r="J68" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K68" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="L68" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B69" s="33">
+        <v>1.3065E-2</v>
+      </c>
+      <c r="C69" s="33">
+        <v>0.17234099999999999</v>
+      </c>
+      <c r="D69" s="33">
+        <v>0.173318</v>
+      </c>
+      <c r="E69" s="33">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F69" s="33">
+        <v>0.93991000000000002</v>
+      </c>
+      <c r="G69" s="2">
+        <v>-1.3698906</v>
+      </c>
+      <c r="H69" s="2">
+        <v>2.3949297000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B70" s="33">
+        <v>6.411E-3</v>
+      </c>
+      <c r="C70" s="33">
+        <v>8.8525999999999994E-2</v>
+      </c>
+      <c r="D70" s="33">
+        <v>8.9038000000000006E-2</v>
+      </c>
+      <c r="E70" s="33">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="F70" s="33">
+        <v>0.94259999999999999</v>
+      </c>
+      <c r="G70" s="2">
+        <v>-0.72881209999999996</v>
+      </c>
+      <c r="H70" s="2">
+        <v>1.2389133999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B71" s="33">
+        <v>-8.7550000000000006E-3</v>
+      </c>
+      <c r="C71" s="33">
+        <v>0.138904</v>
+      </c>
+      <c r="D71" s="33">
+        <v>0.13975099999999999</v>
+      </c>
+      <c r="E71" s="33">
+        <v>6.3E-2</v>
+      </c>
+      <c r="F71" s="33">
+        <v>0.95004999999999995</v>
+      </c>
+      <c r="G71" s="2">
+        <v>-1.9733282000000001</v>
+      </c>
+      <c r="H71" s="2">
+        <v>1.2525704</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+    </row>
+    <row r="73" spans="1:16" s="27" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A73" s="3"/>
+      <c r="B73" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F73" s="3"/>
+      <c r="J73" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B74" s="6">
+        <v>0.26195459999999998</v>
+      </c>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="6">
+        <v>0.29905100000000001</v>
+      </c>
+      <c r="F74" s="6">
+        <v>0.40280660000000001</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J74" s="23">
+        <v>0.27011489999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B75" s="6">
+        <v>0.29639169999999998</v>
+      </c>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="18">
+        <v>0.3310401</v>
+      </c>
+      <c r="F75" s="18">
+        <v>0.44589430000000002</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J75" s="23">
+        <v>0.31034479999999998</v>
+      </c>
+      <c r="P75"/>
+    </row>
+    <row r="76" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P76"/>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A78" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A58" s="13" t="s">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A79" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B58" s="12"/>
-      <c r="C58" s="12" t="s">
+      <c r="B79" s="12"/>
+      <c r="C79" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="12"/>
-      <c r="H58" s="12"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A59" s="14" t="s">
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
+      <c r="H79" s="12"/>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A80" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B59" s="12"/>
-      <c r="C59" s="11" t="s">
+      <c r="B80" s="12"/>
+      <c r="C80" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
-      <c r="H59" s="12"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A60" s="13" t="s">
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="12"/>
+      <c r="H80" s="12"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B60" s="12"/>
-      <c r="C60" s="12" t="s">
+      <c r="B81" s="12"/>
+      <c r="C81" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="12"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A61" s="13" t="s">
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="12"/>
+      <c r="G81" s="12"/>
+      <c r="H81" s="12"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B61" s="12"/>
-      <c r="C61" s="12" t="s">
+      <c r="B82" s="12"/>
+      <c r="C82" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="12"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A63" s="9" t="s">
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
+      <c r="F82" s="12"/>
+      <c r="G82" s="12"/>
+      <c r="H82" s="12"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A64" s="13" t="s">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B64" s="12" t="s">
+      <c r="B85" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
-      <c r="E64" s="12"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="13" t="s">
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B65" s="12" t="s">
+      <c r="B86" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="13" t="s">
+      <c r="C86" s="12"/>
+      <c r="D86" s="12"/>
+      <c r="E86" s="12"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B66" s="12" t="s">
+      <c r="B87" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="13" t="s">
+      <c r="C87" s="12"/>
+      <c r="D87" s="12"/>
+      <c r="E87" s="12"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B67" s="12" t="s">
+      <c r="B88" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="12"/>
+      <c r="C88" s="12"/>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F3:F14">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22:F33">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F22:F33">
+  <conditionalFormatting sqref="F41:F50">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F41:F50">
+  <conditionalFormatting sqref="F58:F71">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
@@ -3589,22 +4226,22 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B37" sqref="B37:B38"/>
+      <selection pane="bottomRight" activeCell="H20" sqref="D17:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.5703125" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="102.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="110.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="20" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="21" customFormat="1" ht="39" x14ac:dyDescent="0.25">
@@ -3620,16 +4257,16 @@
       <c r="D1" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="32" t="s">
         <v>112</v>
       </c>
     </row>
@@ -3739,10 +4376,6 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
@@ -3850,10 +4483,6 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
@@ -3959,40 +4588,141 @@
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C20" s="16"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="C17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" s="20">
+        <v>5</v>
+      </c>
+      <c r="E17" s="20">
+        <v>184.2</v>
+      </c>
+      <c r="F17" s="22">
+        <v>0.26195459999999998</v>
+      </c>
+      <c r="G17" s="22">
+        <v>0.29905100000000001</v>
+      </c>
+      <c r="H17" s="22">
+        <v>0.27011489999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18" s="20">
+        <v>13</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19">
+        <v>14</v>
+      </c>
+      <c r="E19" s="20">
+        <v>194.06</v>
+      </c>
+      <c r="F19" s="22">
+        <v>0.29639169999999998</v>
+      </c>
+      <c r="G19" s="22">
+        <v>0.3310401</v>
+      </c>
+      <c r="H19" s="22">
+        <v>0.31034479999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="20">
+        <v>238.02</v>
+      </c>
+      <c r="F20" s="20">
+        <v>0</v>
+      </c>
+      <c r="G20" s="20">
+        <v>0</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C22" s="16"/>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C23" s="16"/>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C24" s="16"/>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C26" s="16"/>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C27" s="16"/>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C28" s="16"/>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C31" s="16"/>
     </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C32" s="16"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.2">
@@ -4015,15 +4745,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4035,8 +4766,10 @@
     <col min="5" max="5" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="31" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="29"/>
+    <row r="1" spans="1:5" s="31" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="29" t="s">
+        <v>97</v>
+      </c>
       <c r="B1" s="30" t="s">
         <v>38</v>
       </c>
@@ -4085,7 +4818,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" s="27" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="B5" s="30" t="s">
         <v>38</v>
       </c>
@@ -4134,7 +4869,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" s="27" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="B9" s="30" t="s">
         <v>38</v>
       </c>
@@ -4180,6 +4917,11 @@
       </c>
       <c r="E11" s="23">
         <v>0.18390799999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="34" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "lots of glms and spatial correlograms"
This reverts commit 786d4bac25957e16f553fdf91a450d628b26f84a.

Conflicts:
	GLM/all_glm_LM_trans_2.csv
	GLM/all_glm_SP_trans_2.csv
	GLM/all_glm_W_trans_2.csv
	GLM/best_glm_FPpres_trans_partial_resids_plot.jpg
	GLM/best_glm_FPpres_trans_resids_plot.jpg
	GLM/best_glm_FPrich_trans_partial_resids_plot.jpg
	GLM/best_glm_FPrich_trans_resids_plot.jpg
	GLM/glm summary 9-11-2014.xlsx
	code/absences - descriptive stats.R
	code/absences - functional groups - presence in each lake.R
	code/absences - glms - all reponses - transformed.R
	code/absences - transformations.R
	dataSPECIES_freq.csv
	dataSPECIES_freq3_with_func_group_labels.csv
	other regions/sp_freq_plot_CT - with_func_group_labels.jpg
	workspace for plotting other regions - lit.RData
	workspace with all CT data - not a lot of clutter.RData
</commit_message>
<xml_diff>
--- a/GLM/glm summary 9-3-2014.xlsx
+++ b/GLM/glm summary 9-3-2014.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="128">
   <si>
     <t>Estimate</t>
   </si>
@@ -527,21 +527,6 @@
   <si>
     <t>Nagelkerke adjusted</t>
   </si>
-  <si>
-    <t>Fppres</t>
-  </si>
-  <si>
-    <t>cond + longitude + secchi + totalP</t>
-  </si>
-  <si>
-    <t>cond + longitude + secchi + totalP + lakes_1km + pH + latitude + dist_occupied + lakes_10km + waterfowl + boatlaunch + size</t>
-  </si>
-  <si>
-    <t>FP presence/absence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STILL NEED TO ADD FP PRESENCE </t>
-  </si>
 </sst>
 </file>
 
@@ -551,7 +536,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -716,14 +701,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1105,7 +1082,7 @@
     <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1154,11 +1131,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1204,37 +1176,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1566,7 +1508,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1986,15 +1928,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P88"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J75" sqref="J75"/>
+    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="10" customWidth="1"/>
     <col min="9" max="9" width="4.28515625" customWidth="1"/>
@@ -3507,707 +3449,128 @@
         <v>0.18390799999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E57" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F57" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G57" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H57" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J57" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K57" s="8" t="s">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A57" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A58" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="L57" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="B58" s="33">
-        <v>-3.646201</v>
-      </c>
-      <c r="C58" s="33">
-        <v>1.318605</v>
-      </c>
-      <c r="D58" s="33">
-        <v>1.327288</v>
-      </c>
-      <c r="E58" s="33">
-        <v>2.7469999999999999</v>
-      </c>
-      <c r="F58" s="33">
-        <v>6.0099999999999997E-3</v>
-      </c>
-      <c r="G58" s="2">
-        <v>-6.2476381999999999</v>
-      </c>
-      <c r="H58" s="2">
-        <v>-1.0447637999999999</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K58" s="2">
-        <v>1</v>
-      </c>
-      <c r="L58" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="B59" s="33">
-        <v>3.5329160000000002</v>
-      </c>
-      <c r="C59" s="33">
-        <v>1.2057100000000001</v>
-      </c>
-      <c r="D59" s="33">
-        <v>1.213508</v>
-      </c>
-      <c r="E59" s="33">
-        <v>2.911</v>
-      </c>
-      <c r="F59" s="33">
-        <v>3.5999999999999999E-3</v>
-      </c>
-      <c r="G59" s="2">
-        <v>1.1544836999999999</v>
-      </c>
-      <c r="H59" s="2">
-        <v>5.9113480000000003</v>
-      </c>
-      <c r="J59" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K59" s="2">
-        <v>1</v>
-      </c>
-      <c r="L59" s="2">
+      <c r="B58" s="12"/>
+      <c r="C58" s="12" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B60" s="33">
-        <v>0.54410599999999998</v>
-      </c>
-      <c r="C60" s="33">
-        <v>0.80477100000000001</v>
-      </c>
-      <c r="D60" s="33">
-        <v>0.80750100000000002</v>
-      </c>
-      <c r="E60" s="33">
-        <v>0.67400000000000004</v>
-      </c>
-      <c r="F60" s="33">
-        <v>0.50043000000000004</v>
-      </c>
-      <c r="G60" s="2">
-        <v>-0.42544359999999998</v>
-      </c>
-      <c r="H60" s="2">
-        <v>2.7754997000000001</v>
-      </c>
-      <c r="J60" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K60" s="2">
-        <v>1</v>
-      </c>
-      <c r="L60" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="B61" s="33">
-        <v>-2.7370329999999998</v>
-      </c>
-      <c r="C61" s="33">
-        <v>1.2762169999999999</v>
-      </c>
-      <c r="D61" s="33">
-        <v>1.2853889999999999</v>
-      </c>
-      <c r="E61" s="33">
-        <v>2.129</v>
-      </c>
-      <c r="F61" s="33">
-        <v>3.3230000000000003E-2</v>
-      </c>
-      <c r="G61" s="2">
-        <v>-5.2563493000000001</v>
-      </c>
-      <c r="H61" s="2">
-        <v>-0.21771599999999999</v>
-      </c>
-      <c r="J61" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K61" s="2">
-        <v>0.46</v>
-      </c>
-      <c r="L61" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="B62" s="33">
-        <v>4.739579</v>
-      </c>
-      <c r="C62" s="33">
-        <v>1.5687409999999999</v>
-      </c>
-      <c r="D62" s="33">
-        <v>1.5799730000000001</v>
-      </c>
-      <c r="E62" s="33">
-        <v>3</v>
-      </c>
-      <c r="F62" s="33">
-        <v>2.7000000000000001E-3</v>
-      </c>
-      <c r="G62" s="2">
-        <v>1.6428894999999999</v>
-      </c>
-      <c r="H62" s="2">
-        <v>7.8362691</v>
-      </c>
-      <c r="J62" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K62" s="2">
-        <v>0.34</v>
-      </c>
-      <c r="L62" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="B63" s="33">
-        <v>-0.33143099999999998</v>
-      </c>
-      <c r="C63" s="33">
-        <v>0.63272399999999995</v>
-      </c>
-      <c r="D63" s="33">
-        <v>0.63486900000000002</v>
-      </c>
-      <c r="E63" s="33">
-        <v>0.52200000000000002</v>
-      </c>
-      <c r="F63" s="33">
-        <v>0.60163999999999995</v>
-      </c>
-      <c r="G63" s="2">
-        <v>-2.4361264999999999</v>
-      </c>
-      <c r="H63" s="2">
-        <v>0.49967289999999998</v>
-      </c>
-      <c r="J63" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K63" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="L63" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="B64" s="33">
-        <v>0.40556999999999999</v>
-      </c>
-      <c r="C64" s="33">
-        <v>1.015307</v>
-      </c>
-      <c r="D64" s="33">
-        <v>1.018883</v>
-      </c>
-      <c r="E64" s="33">
-        <v>0.39800000000000002</v>
-      </c>
-      <c r="F64" s="33">
-        <v>0.69059000000000004</v>
-      </c>
-      <c r="G64" s="2">
-        <v>-1.1825922</v>
-      </c>
-      <c r="H64" s="2">
-        <v>4.5699639999999997</v>
-      </c>
-      <c r="J64" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K64" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="L64" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="B65" s="33">
-        <v>-0.24573200000000001</v>
-      </c>
-      <c r="C65" s="33">
-        <v>0.60241800000000001</v>
-      </c>
-      <c r="D65" s="33">
-        <v>0.60433599999999998</v>
-      </c>
-      <c r="E65" s="33">
-        <v>0.40699999999999997</v>
-      </c>
-      <c r="F65" s="33">
-        <v>0.68428999999999995</v>
-      </c>
-      <c r="G65" s="2">
-        <v>-2.6903693</v>
-      </c>
-      <c r="H65" s="2">
-        <v>0.65005389999999996</v>
-      </c>
-      <c r="J65" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="K65" s="2">
-        <v>0.16</v>
-      </c>
-      <c r="L65" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="B66" s="33">
-        <v>0.18145800000000001</v>
-      </c>
-      <c r="C66" s="33">
-        <v>0.57772000000000001</v>
-      </c>
-      <c r="D66" s="33">
-        <v>0.57954799999999995</v>
-      </c>
-      <c r="E66" s="33">
-        <v>0.313</v>
-      </c>
-      <c r="F66" s="33">
-        <v>0.75419999999999998</v>
-      </c>
-      <c r="G66" s="2">
-        <v>-0.80408670000000004</v>
-      </c>
-      <c r="H66" s="2">
-        <v>3.1359618999999999</v>
-      </c>
-      <c r="J66" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K66" s="2">
-        <v>0.16</v>
-      </c>
-      <c r="L66" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="B67" s="33">
-        <v>0.18346299999999999</v>
-      </c>
-      <c r="C67" s="33">
-        <v>0.59925499999999998</v>
-      </c>
-      <c r="D67" s="33">
-        <v>0.601329</v>
-      </c>
-      <c r="E67" s="33">
-        <v>0.30499999999999999</v>
-      </c>
-      <c r="F67" s="33">
-        <v>0.76029000000000002</v>
-      </c>
-      <c r="G67" s="2">
-        <v>-0.92119720000000005</v>
-      </c>
-      <c r="H67" s="2">
-        <v>3.2819623999999998</v>
-      </c>
-      <c r="J67" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K67" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="L67" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="B68" s="33">
-        <v>0.11201999999999999</v>
-      </c>
-      <c r="C68" s="33">
-        <v>0.44223200000000001</v>
-      </c>
-      <c r="D68" s="33">
-        <v>0.443913</v>
-      </c>
-      <c r="E68" s="33">
-        <v>0.252</v>
-      </c>
-      <c r="F68" s="33">
-        <v>0.80076999999999998</v>
-      </c>
-      <c r="G68" s="2">
-        <v>-0.90429159999999997</v>
-      </c>
-      <c r="H68" s="2">
-        <v>2.7630219999999999</v>
-      </c>
-      <c r="J68" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K68" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="L68" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B69" s="33">
-        <v>1.3065E-2</v>
-      </c>
-      <c r="C69" s="33">
-        <v>0.17234099999999999</v>
-      </c>
-      <c r="D69" s="33">
-        <v>0.173318</v>
-      </c>
-      <c r="E69" s="33">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="F69" s="33">
-        <v>0.93991000000000002</v>
-      </c>
-      <c r="G69" s="2">
-        <v>-1.3698906</v>
-      </c>
-      <c r="H69" s="2">
-        <v>2.3949297000000001</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="B70" s="33">
-        <v>6.411E-3</v>
-      </c>
-      <c r="C70" s="33">
-        <v>8.8525999999999994E-2</v>
-      </c>
-      <c r="D70" s="33">
-        <v>8.9038000000000006E-2</v>
-      </c>
-      <c r="E70" s="33">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="F70" s="33">
-        <v>0.94259999999999999</v>
-      </c>
-      <c r="G70" s="2">
-        <v>-0.72881209999999996</v>
-      </c>
-      <c r="H70" s="2">
-        <v>1.2389133999999999</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="B71" s="33">
-        <v>-8.7550000000000006E-3</v>
-      </c>
-      <c r="C71" s="33">
-        <v>0.138904</v>
-      </c>
-      <c r="D71" s="33">
-        <v>0.13975099999999999</v>
-      </c>
-      <c r="E71" s="33">
-        <v>6.3E-2</v>
-      </c>
-      <c r="F71" s="33">
-        <v>0.95004999999999995</v>
-      </c>
-      <c r="G71" s="2">
-        <v>-1.9733282000000001</v>
-      </c>
-      <c r="H71" s="2">
-        <v>1.2525704</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="3"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-    </row>
-    <row r="73" spans="1:16" s="27" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A73" s="3"/>
-      <c r="B73" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F73" s="3"/>
-      <c r="J73" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="5" t="s">
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A59" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59" s="12"/>
+      <c r="C59" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A60" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B74" s="6">
-        <v>0.26195459999999998</v>
-      </c>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="6">
-        <v>0.29905100000000001</v>
-      </c>
-      <c r="F74" s="6">
-        <v>0.40280660000000001</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J74" s="23">
-        <v>0.27011489999999999</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B75" s="6">
-        <v>0.29639169999999998</v>
-      </c>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="18">
-        <v>0.3310401</v>
-      </c>
-      <c r="F75" s="18">
-        <v>0.44589430000000002</v>
-      </c>
-      <c r="G75" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J75" s="23">
-        <v>0.31034479999999998</v>
-      </c>
-      <c r="P75"/>
-    </row>
-    <row r="76" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="P76"/>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A78" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A79" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B79" s="12"/>
-      <c r="C79" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D79" s="12"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="12"/>
-      <c r="G79" s="12"/>
-      <c r="H79" s="12"/>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A80" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B80" s="12"/>
-      <c r="C80" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D80" s="12"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
-      <c r="G80" s="12"/>
-      <c r="H80" s="12"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B81" s="12"/>
-      <c r="C81" s="12" t="s">
+      <c r="B60" s="12"/>
+      <c r="C60" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D81" s="12"/>
-      <c r="E81" s="12"/>
-      <c r="F81" s="12"/>
-      <c r="G81" s="12"/>
-      <c r="H81" s="12"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="13" t="s">
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A61" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B82" s="12"/>
-      <c r="C82" s="12" t="s">
+      <c r="B61" s="12"/>
+      <c r="C61" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D82" s="12"/>
-      <c r="E82" s="12"/>
-      <c r="F82" s="12"/>
-      <c r="G82" s="12"/>
-      <c r="H82" s="12"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="9" t="s">
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="12"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A63" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="13" t="s">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A64" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B85" s="12" t="s">
+      <c r="B64" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C85" s="12"/>
-      <c r="D85" s="12"/>
-      <c r="E85" s="12"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="13" t="s">
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B86" s="12" t="s">
+      <c r="B65" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C86" s="12"/>
-      <c r="D86" s="12"/>
-      <c r="E86" s="12"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="13" t="s">
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B87" s="12" t="s">
+      <c r="B66" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C87" s="12"/>
-      <c r="D87" s="12"/>
-      <c r="E87" s="12"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" s="13" t="s">
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B88" s="12" t="s">
+      <c r="B67" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C88" s="12"/>
-      <c r="D88" s="12"/>
-      <c r="E88" s="12"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F3:F14">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22:F33">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F41:F50">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
-      <formula>0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F58:F71">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
@@ -4226,22 +3589,22 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H20" sqref="D17:H20"/>
+      <selection pane="bottomRight" activeCell="B37" sqref="B37:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.5703125" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="110.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="102.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="20" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="21" customFormat="1" ht="39" x14ac:dyDescent="0.25">
@@ -4257,16 +3620,16 @@
       <c r="D1" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="28" t="s">
         <v>112</v>
       </c>
     </row>
@@ -4376,6 +3739,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
@@ -4483,6 +3850,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
@@ -4588,141 +3959,40 @@
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="B17" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="C17" t="s">
-        <v>129</v>
-      </c>
-      <c r="D17" s="20">
-        <v>5</v>
-      </c>
-      <c r="E17" s="20">
-        <v>184.2</v>
-      </c>
-      <c r="F17" s="22">
-        <v>0.26195459999999998</v>
-      </c>
-      <c r="G17" s="22">
-        <v>0.29905100000000001</v>
-      </c>
-      <c r="H17" s="22">
-        <v>0.27011489999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="B18" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="C18" t="s">
-        <v>130</v>
-      </c>
-      <c r="D18" s="20">
-        <v>13</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="H18" s="20" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="B19" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="D19">
-        <v>14</v>
-      </c>
-      <c r="E19" s="20">
-        <v>194.06</v>
-      </c>
-      <c r="F19" s="22">
-        <v>0.29639169999999998</v>
-      </c>
-      <c r="G19" s="22">
-        <v>0.3310401</v>
-      </c>
-      <c r="H19" s="22">
-        <v>0.31034479999999998</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="B20" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="C20" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" s="20">
-        <v>238.02</v>
-      </c>
-      <c r="F20" s="20">
-        <v>0</v>
-      </c>
-      <c r="G20" s="20">
-        <v>0</v>
-      </c>
-      <c r="H20" s="20" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C20" s="16"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C22" s="16"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C23" s="16"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C24" s="16"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C26" s="16"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C27" s="16"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C28" s="16"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C31" s="16"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C32" s="16"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.2">
@@ -4745,16 +4015,15 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4766,10 +4035,8 @@
     <col min="5" max="5" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="31" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
-        <v>97</v>
-      </c>
+    <row r="1" spans="1:5" s="31" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="29"/>
       <c r="B1" s="30" t="s">
         <v>38</v>
       </c>
@@ -4818,9 +4085,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" s="27" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>98</v>
-      </c>
+      <c r="A5" s="3"/>
       <c r="B5" s="30" t="s">
         <v>38</v>
       </c>
@@ -4869,9 +4134,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" s="27" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>99</v>
-      </c>
+      <c r="A9" s="3"/>
       <c r="B9" s="30" t="s">
         <v>38</v>
       </c>
@@ -4917,11 +4180,6 @@
       </c>
       <c r="E11" s="23">
         <v>0.18390799999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="34" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>